<commit_message>
Menu update DSL Editor fields QA and classification completion
</commit_message>
<xml_diff>
--- a/debug config.xlsx
+++ b/debug config.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="137">
   <si>
     <t>Connexion =&gt; Connection</t>
   </si>
@@ -435,6 +435,9 @@
   </si>
   <si>
     <t>On utiliser le doigt pour scroll</t>
+  </si>
+  <si>
+    <t>Enle</t>
   </si>
 </sst>
 </file>
@@ -960,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE98B639-DF19-4567-86E5-F5665EF5CE3E}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,6 +1591,11 @@
       </c>
       <c r="C58" s="3" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>